<commit_message>
fix bug, when loop, add null if not exist (0kg)
</commit_message>
<xml_diff>
--- a/tong-hop.xlsx
+++ b/tong-hop.xlsx
@@ -10,14 +10,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="6">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@"/>
-    <numFmt numFmtId="166" formatCode="00"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ _₫_-;\-* #,##0.00\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
-  </numFmts>
   <fonts count="1">
     <font>
       <sz val="12"/>
@@ -380,25 +372,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:C64"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
         <v>Tên sản phẩm</v>
       </c>
       <c r="B1" t="str">
-        <v>Mon Sep 19 2016 09:00:48 GMT+0700 (SE Asia Standard Time)</v>
+        <v>Mon Sep 19 2016 16:12:26 GMT+0700 (SE Asia Standard Time)</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" t="str">
-        <v>3 sạch 17_09_2016.xlsx</v>
+        <v>3 sạch 17_09_2016</v>
       </c>
       <c r="C2" t="str">
-        <v>HQ Food..xlsx</v>
-      </c>
-      <c r="D2" t="str">
-        <v>Đơn hàng VFFM.xlsx</v>
+        <v>HQ Food.</v>
       </c>
     </row>
     <row r="3">
@@ -410,11 +399,8 @@
       <c r="A4" t="str">
         <v>Xà lách lolo tím</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>1</v>
-      </c>
-      <c r="C4">
-        <v>0.6</v>
       </c>
     </row>
     <row r="5">
@@ -427,38 +413,23 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
         <v>Xà lách Romaine</v>
       </c>
-      <c r="B6">
-        <v>0.5</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
         <v>Xà lách Oakleaf xanh</v>
       </c>
-      <c r="B7">
-        <v>0.6</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
         <v>Xà lách IceBerg</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>1</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -470,9 +441,6 @@
       <c r="A10" t="str">
         <v>Xà lách Mỡ</v>
       </c>
-      <c r="B10">
-        <v>0.78</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -486,17 +454,11 @@
       <c r="B12">
         <v>30</v>
       </c>
-      <c r="C12">
-        <v>2.5</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
         <v>Cà chua Beef</v>
       </c>
-      <c r="B13">
-        <v>1.3</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -512,11 +474,8 @@
       <c r="A16" t="str">
         <v>Cà chua Doufu</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>5</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
       </c>
     </row>
     <row r="17">
@@ -539,12 +498,6 @@
       <c r="C19">
         <v>3</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>2.5</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -555,30 +508,18 @@
       <c r="A21" t="str">
         <v>Cà chua bi socola 250gr</v>
       </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
         <v>Cà chua bi socola 500gr</v>
       </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
         <v>Dưa Leo baby</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>4</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -588,12 +529,6 @@
       <c r="B24">
         <v>15</v>
       </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -605,46 +540,16 @@
       <c r="C25">
         <v>6</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>4</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
         <v>Bí Đỏ hồ lô</v>
       </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
         <v>Cải Thảo</v>
       </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <v>3</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
@@ -655,12 +560,6 @@
       <c r="A29" t="str">
         <v>Su Su</v>
       </c>
-      <c r="B29">
-        <v>1.5</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
@@ -671,9 +570,6 @@
       <c r="A31" t="str">
         <v>Chanh Dây</v>
       </c>
-      <c r="B31">
-        <v>1.6</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -690,9 +586,6 @@
       <c r="A33" t="str">
         <v>Bó Xôi mini</v>
       </c>
-      <c r="B33">
-        <v>3</v>
-      </c>
       <c r="C33">
         <v>3</v>
       </c>
@@ -706,134 +599,86 @@
       <c r="A35" t="str">
         <v>Khoai tây vàng</v>
       </c>
-      <c r="B35">
-        <v>3</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
         <v>Khoai tây hồng</v>
       </c>
-      <c r="B36">
-        <v>0</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
         <v>Cà Rốt</v>
       </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
         <v>Cà rốt mini</v>
       </c>
-      <c r="B38">
+      <c r="C38">
         <v>1</v>
-      </c>
-      <c r="C38">
-        <v>2.1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
         <v>Cà rốt Đà Lạt</v>
       </c>
-      <c r="B39">
+      <c r="C39">
         <v>1</v>
-      </c>
-      <c r="C39">
-        <v>1.5</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
         <v>Củ Dền</v>
       </c>
-      <c r="B40">
-        <v>1.75</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
         <v>Rau Gia Vị</v>
       </c>
-      <c r="B41">
-        <v>0</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
         <v>Súp Lơ Xanh mini</v>
       </c>
-      <c r="B42">
+      <c r="C42">
         <v>5</v>
-      </c>
-      <c r="C42">
-        <v>1.8</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
         <v>Bắp Cải</v>
       </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
         <v>Bắp cải trắng</v>
       </c>
-      <c r="B44">
+      <c r="C44">
         <v>1</v>
-      </c>
-      <c r="C44">
-        <v>5.6</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
         <v>Bắp cải trái tim</v>
       </c>
-      <c r="B45">
+      <c r="C45">
         <v>3</v>
-      </c>
-      <c r="C45">
-        <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
         <v>Bắp cải mini giống Nhật</v>
       </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
         <v>Cải Thìa</v>
       </c>
-      <c r="B47">
-        <v>1.5</v>
-      </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
         <v>Cải Cầu Vồng</v>
       </c>
-      <c r="B48">
-        <v>0.6</v>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
@@ -849,12 +694,6 @@
       <c r="A51" t="str">
         <v>Ớt Chuông baby</v>
       </c>
-      <c r="B51">
-        <v>0</v>
-      </c>
-      <c r="C51">
-        <v>0</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
@@ -870,17 +709,11 @@
       <c r="A54" t="str">
         <v>Hành lá</v>
       </c>
-      <c r="B54">
-        <v>2</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
         <v>Hành Paro</v>
       </c>
-      <c r="B55">
-        <v>0</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
@@ -891,71 +724,44 @@
       <c r="A57" t="str">
         <v>Chanh không hạt</v>
       </c>
-      <c r="B57">
-        <v>2.1</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
         <v>Củ cải đỏ</v>
       </c>
-      <c r="B58">
-        <v>1.5</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
         <v>Hành tây</v>
       </c>
-      <c r="B59">
-        <v>5</v>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
         <v>Nấm Ngọc Thạch Đà Lạt</v>
       </c>
-      <c r="B60">
-        <v>0</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
         <v>Bí Xanh non</v>
       </c>
-      <c r="B61">
-        <v>0</v>
-      </c>
-      <c r="C61">
-        <v>0</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
         <v>Bí Ngòi Xanh</v>
       </c>
-      <c r="B62">
+      <c r="C62">
         <v>4</v>
-      </c>
-      <c r="C62">
-        <v>5</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
         <v>Gừng</v>
       </c>
-      <c r="B63">
-        <v>2</v>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
         <v>Củ cải trắng</v>
       </c>
-      <c r="B64">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
commit before 'significant' change, v2
</commit_message>
<xml_diff>
--- a/tong-hop.xlsx
+++ b/tong-hop.xlsx
@@ -372,21 +372,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:B64"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
         <v>Tên sản phẩm</v>
       </c>
       <c r="B1" t="str">
-        <v>Mon Sep 19 2016 16:12:26 GMT+0700 (SE Asia Standard Time)</v>
+        <v>Wed Sep 21 2016 15:31:21 GMT+0700 (SE Asia Standard Time)</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" t="str">
-        <v>3 sạch 17_09_2016</v>
-      </c>
-      <c r="C2" t="str">
         <v>HQ Food.</v>
       </c>
     </row>
@@ -399,7 +396,7 @@
       <c r="A4" t="str">
         <v>Xà lách lolo tím</v>
       </c>
-      <c r="C4">
+      <c r="B4">
         <v>1</v>
       </c>
     </row>
@@ -408,9 +405,6 @@
         <v>Xà lách lolo xanh</v>
       </c>
       <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
         <v>1</v>
       </c>
     </row>
@@ -428,7 +422,7 @@
       <c r="A8" t="str">
         <v>Xà lách IceBerg</v>
       </c>
-      <c r="C8">
+      <c r="B8">
         <v>1</v>
       </c>
     </row>
@@ -451,9 +445,6 @@
       <c r="A12" t="str">
         <v>Cà chua Đà Lạt</v>
       </c>
-      <c r="B12">
-        <v>30</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -474,7 +465,7 @@
       <c r="A16" t="str">
         <v>Cà chua Doufu</v>
       </c>
-      <c r="C16">
+      <c r="B16">
         <v>5</v>
       </c>
     </row>
@@ -493,9 +484,6 @@
         <v>Cà chua Picota 250gr</v>
       </c>
       <c r="B19">
-        <v>5</v>
-      </c>
-      <c r="C19">
         <v>3</v>
       </c>
     </row>
@@ -518,7 +506,7 @@
       <c r="A23" t="str">
         <v>Dưa Leo baby</v>
       </c>
-      <c r="C23">
+      <c r="B23">
         <v>4</v>
       </c>
     </row>
@@ -526,18 +514,12 @@
       <c r="A24" t="str">
         <v>Khoai Lang mật</v>
       </c>
-      <c r="B24">
-        <v>15</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
         <v>Chuối Laba</v>
       </c>
       <c r="B25">
-        <v>15</v>
-      </c>
-      <c r="C25">
         <v>6</v>
       </c>
     </row>
@@ -576,9 +558,6 @@
         <v>Lá trà xanh</v>
       </c>
       <c r="B32">
-        <v>1.5</v>
-      </c>
-      <c r="C32">
         <v>5</v>
       </c>
     </row>
@@ -586,7 +565,7 @@
       <c r="A33" t="str">
         <v>Bó Xôi mini</v>
       </c>
-      <c r="C33">
+      <c r="B33">
         <v>3</v>
       </c>
     </row>
@@ -614,7 +593,7 @@
       <c r="A38" t="str">
         <v>Cà rốt mini</v>
       </c>
-      <c r="C38">
+      <c r="B38">
         <v>1</v>
       </c>
     </row>
@@ -622,7 +601,7 @@
       <c r="A39" t="str">
         <v>Cà rốt Đà Lạt</v>
       </c>
-      <c r="C39">
+      <c r="B39">
         <v>1</v>
       </c>
     </row>
@@ -640,7 +619,7 @@
       <c r="A42" t="str">
         <v>Súp Lơ Xanh mini</v>
       </c>
-      <c r="C42">
+      <c r="B42">
         <v>5</v>
       </c>
     </row>
@@ -653,7 +632,7 @@
       <c r="A44" t="str">
         <v>Bắp cải trắng</v>
       </c>
-      <c r="C44">
+      <c r="B44">
         <v>1</v>
       </c>
     </row>
@@ -661,7 +640,7 @@
       <c r="A45" t="str">
         <v>Bắp cải trái tim</v>
       </c>
-      <c r="C45">
+      <c r="B45">
         <v>3</v>
       </c>
     </row>
@@ -749,7 +728,7 @@
       <c r="A62" t="str">
         <v>Bí Ngòi Xanh</v>
       </c>
-      <c r="C62">
+      <c r="B62">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dev2 branch, for simplicity, just work better, NO watcher, NO learning, check out dev2
</commit_message>
<xml_diff>
--- a/tong-hop.xlsx
+++ b/tong-hop.xlsx
@@ -10,6 +10,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="11">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0;\-&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="12"/>
@@ -372,22 +385,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:I64"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
         <v>Tên sản phẩm</v>
       </c>
       <c r="B1" t="str">
-        <v>Mon Sep 19 2016 16:12:26 GMT+0700 (SE Asia Standard Time)</v>
+        <v>Sun Sep 25 2016 00:08:20 GMT+0700 (SE Asia Standard Time)</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" t="str">
+        <v>product</v>
+      </c>
+      <c r="C2" t="str">
         <v>3 sạch 17_09_2016</v>
       </c>
-      <c r="C2" t="str">
-        <v>HQ Food.</v>
+      <c r="D2" t="str">
+        <v>product</v>
+      </c>
+      <c r="E2" t="str">
+        <v>3sis mart</v>
+      </c>
+      <c r="F2" t="str">
+        <v>product</v>
+      </c>
+      <c r="G2" t="str">
+        <v>Hello măm.xls</v>
       </c>
     </row>
     <row r="3">
@@ -399,19 +424,16 @@
       <c r="A4" t="str">
         <v>Xà lách lolo tím</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
         <v>Xà lách lolo xanh</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="str">
+        <v xml:space="preserve">Xà lách lolo xanh </v>
+      </c>
+      <c r="C5">
         <v>3</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -428,8 +450,11 @@
       <c r="A8" t="str">
         <v>Xà lách IceBerg</v>
       </c>
-      <c r="C8">
-        <v>1</v>
+      <c r="F8" t="str">
+        <v>Xà lách Ice Berg</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -441,6 +466,12 @@
       <c r="A10" t="str">
         <v>Xà lách Mỡ</v>
       </c>
+      <c r="D10" t="str">
+        <v>Xà lách Mỡ</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -451,8 +482,17 @@
       <c r="A12" t="str">
         <v>Cà chua Đà Lạt</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="str">
+        <v>Cà chua Hà Lan</v>
+      </c>
+      <c r="C12">
         <v>30</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Cà chua Hà Lan</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
       </c>
     </row>
     <row r="13">
@@ -474,9 +514,6 @@
       <c r="A16" t="str">
         <v>Cà chua Doufu</v>
       </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -492,11 +529,23 @@
       <c r="A19" t="str">
         <v>Cà chua Picota 250gr</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="str">
+        <v>Cà chua socola - 500gr</v>
+      </c>
+      <c r="C19">
         <v>5</v>
       </c>
-      <c r="C19">
-        <v>3</v>
+      <c r="D19" t="str">
+        <v>Cà chua picota 250gr</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" t="str">
+        <v>Cà chua picota 250 gr</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
       </c>
     </row>
     <row r="20">
@@ -518,27 +567,57 @@
       <c r="A23" t="str">
         <v>Dưa Leo baby</v>
       </c>
-      <c r="C23">
-        <v>4</v>
+      <c r="D23" t="str">
+        <v>Dưa leo baby</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
         <v>Khoai Lang mật</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="str">
+        <v>Khoai lang mật</v>
+      </c>
+      <c r="C24">
         <v>15</v>
+      </c>
+      <c r="D24" t="str">
+        <v>Khoai lang</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24" t="str">
+        <v>Khoai lang nhật 1kg</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
         <v>Chuối Laba</v>
       </c>
-      <c r="B25">
+      <c r="B25" t="str">
+        <v>Chuối laba Đà Lạt 1kg</v>
+      </c>
+      <c r="C25">
         <v>15</v>
       </c>
-      <c r="C25">
-        <v>6</v>
+      <c r="D25" t="str">
+        <v>Chuối Laba Đà Lạt 1kg</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25" t="str">
+        <v>Chuối laba 1kg</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
       </c>
     </row>
     <row r="26">
@@ -555,11 +634,29 @@
       <c r="A28" t="str">
         <v>Dâu Tây</v>
       </c>
+      <c r="F28" t="str">
+        <v>Dâu tây Newzealand</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28" t="str">
+        <v>Dâu tây giống Pháp</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
         <v>Su Su</v>
       </c>
+      <c r="F29" t="str">
+        <v>Su su non 400gr</v>
+      </c>
+      <c r="G29">
+        <v>3</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
@@ -575,20 +672,17 @@
       <c r="A32" t="str">
         <v>Lá trà xanh</v>
       </c>
-      <c r="B32">
+      <c r="B32" t="str">
+        <v xml:space="preserve">Lá trà xanh </v>
+      </c>
+      <c r="C32">
         <v>1.5</v>
-      </c>
-      <c r="C32">
-        <v>5</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
         <v>Bó Xôi mini</v>
       </c>
-      <c r="C33">
-        <v>3</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
@@ -599,6 +693,18 @@
       <c r="A35" t="str">
         <v>Khoai tây vàng</v>
       </c>
+      <c r="D35" t="str">
+        <v>Khoai tây vàng</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" t="str">
+        <v>Khoai tây vàng</v>
+      </c>
+      <c r="G35">
+        <v>4</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
@@ -614,16 +720,16 @@
       <c r="A38" t="str">
         <v>Cà rốt mini</v>
       </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
         <v>Cà rốt Đà Lạt</v>
       </c>
-      <c r="C39">
-        <v>1</v>
+      <c r="F39" t="str">
+        <v xml:space="preserve">Cà rốt đà lạt </v>
+      </c>
+      <c r="G39">
+        <v>5</v>
       </c>
     </row>
     <row r="40">
@@ -640,8 +746,11 @@
       <c r="A42" t="str">
         <v>Súp Lơ Xanh mini</v>
       </c>
-      <c r="C42">
-        <v>5</v>
+      <c r="F42" t="str">
+        <v xml:space="preserve">Súp lơ xanh mini </v>
+      </c>
+      <c r="G42">
+        <v>3</v>
       </c>
     </row>
     <row r="43">
@@ -653,16 +762,22 @@
       <c r="A44" t="str">
         <v>Bắp cải trắng</v>
       </c>
-      <c r="C44">
-        <v>1</v>
+      <c r="D44" t="str">
+        <v>Bắp cải trắng</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
         <v>Bắp cải trái tim</v>
       </c>
-      <c r="C45">
-        <v>3</v>
+      <c r="F45" t="str">
+        <v>Bắp cải trái tim</v>
+      </c>
+      <c r="G45">
+        <v>2</v>
       </c>
     </row>
     <row r="46">
@@ -679,6 +794,12 @@
       <c r="A48" t="str">
         <v>Cải Cầu Vồng</v>
       </c>
+      <c r="D48" t="str">
+        <v>Cải cầu vồng</v>
+      </c>
+      <c r="E48">
+        <v>5</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
@@ -709,6 +830,12 @@
       <c r="A54" t="str">
         <v>Hành lá</v>
       </c>
+      <c r="F54" t="str">
+        <v>Hành lá</v>
+      </c>
+      <c r="G54">
+        <v>4</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
@@ -719,11 +846,23 @@
       <c r="A56" t="str">
         <v>Sả</v>
       </c>
+      <c r="F56" t="str">
+        <v>Sả cây</v>
+      </c>
+      <c r="G56">
+        <v>12</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
         <v>Chanh không hạt</v>
       </c>
+      <c r="F57" t="str">
+        <v xml:space="preserve">Chanh không hạt </v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
@@ -749,14 +888,23 @@
       <c r="A62" t="str">
         <v>Bí Ngòi Xanh</v>
       </c>
-      <c r="C62">
-        <v>4</v>
+      <c r="F62" t="str">
+        <v>Bí ngòi xanh</v>
+      </c>
+      <c r="G62">
+        <v>2</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
         <v>Gừng</v>
       </c>
+      <c r="F63" t="str">
+        <v>Gừng</v>
+      </c>
+      <c r="G63">
+        <v>2</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="str">

</xml_diff>